<commit_message>
Add additional location, update battery sizes, correct load outputs
</commit_message>
<xml_diff>
--- a/Studies/Haiti_USAID/Coordinates for Representative Microgrid Towns.xlsx
+++ b/Studies/Haiti_USAID/Coordinates for Representative Microgrid Towns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmirletz\source\repos\InSPIRE\Studies\Haiti_USAID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAF06087-09C0-4731-9D2B-DB681FFD53F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991483A3-6202-4F98-A001-E56D985FB4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31A8581E-71AA-4225-AA92-9DFCD9B87D9D}"/>
+    <workbookView xWindow="3285" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{31A8581E-71AA-4225-AA92-9DFCD9B87D9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Agrivoltaics Archetype</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Cornillon</t>
+  </si>
+  <si>
+    <t>Nord-Est</t>
+  </si>
+  <si>
+    <t>Perches</t>
   </si>
 </sst>
 </file>
@@ -158,10 +164,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -478,26 +487,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B42BEC-5284-4A99-BC49-77169E438016}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -537,7 +546,7 @@
         <v>156617</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -557,7 +566,7 @@
         <v>170021</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -577,7 +586,7 @@
         <v>169865</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -605,7 +614,7 @@
         <v>164949.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -625,7 +634,7 @@
         <v>177611</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -645,7 +654,7 @@
         <v>162151</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -662,41 +671,58 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3">
+        <v>19.516156630000001</v>
+      </c>
+      <c r="D9" s="3">
+        <v>-71.937673329999996</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>18.750300939999999</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
         <v>-71.826720050000006</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H10" s="1">
         <f>G6/G2</f>
         <v>1.1340467509912717</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>18.710992210000001</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>-71.957197179999994</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -706,6 +732,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e17f2b51-a4e7-4f56-9066-67183771fee9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a39b28b-136c-4db3-a983-7c4ac4e88244">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006364AC3710A7054B9C970042B64DE5EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f97f2e955e9951898cb93c9ef8f237e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a39b28b-136c-4db3-a983-7c4ac4e88244" xmlns:ns3="e17f2b51-a4e7-4f56-9066-67183771fee9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="001a2f3fba6f0e5729002202fa881b5c" ns2:_="" ns3:_="">
     <xsd:import namespace="9a39b28b-136c-4db3-a983-7c4ac4e88244"/>
@@ -928,27 +974,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09C4C47D-2E65-4A4F-99E8-B6FA7AEB788D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9a39b28b-136c-4db3-a983-7c4ac4e88244"/>
+    <ds:schemaRef ds:uri="e17f2b51-a4e7-4f56-9066-67183771fee9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e17f2b51-a4e7-4f56-9066-67183771fee9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a39b28b-136c-4db3-a983-7c4ac4e88244">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B76F7606-34E6-4C2E-9332-0B1C2A81C25E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C08F30E7-F823-4141-B67B-C4B1DDE4F9CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -965,29 +1016,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B76F7606-34E6-4C2E-9332-0B1C2A81C25E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09C4C47D-2E65-4A4F-99E8-B6FA7AEB788D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9a39b28b-136c-4db3-a983-7c4ac4e88244"/>
-    <ds:schemaRef ds:uri="e17f2b51-a4e7-4f56-9066-67183771fee9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>